<commit_message>
Se ajusta funcionalidad para mostrar las informacion segun los filtros
</commit_message>
<xml_diff>
--- a/service/Resources/Base-pilos.xlsx
+++ b/service/Resources/Base-pilos.xlsx
@@ -5373,11 +5373,12 @@
   <dimension ref="A1:I1206"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="19.125" customWidth="1"/>
     <col min="7" max="7" width="22.875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="71.5" customWidth="1"/>
@@ -8109,7 +8110,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A95" s="42" t="s">
         <v>159</v>
       </c>
@@ -8138,7 +8139,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A96" s="42" t="s">
         <v>159</v>
       </c>
@@ -8167,7 +8168,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A97" s="42" t="s">
         <v>159</v>
       </c>
@@ -8196,7 +8197,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A98" s="42" t="s">
         <v>159</v>
       </c>
@@ -8225,7 +8226,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A99" s="42" t="s">
         <v>159</v>
       </c>
@@ -8254,7 +8255,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A100" s="42" t="s">
         <v>159</v>
       </c>
@@ -8283,7 +8284,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A101" s="42" t="s">
         <v>159</v>
       </c>
@@ -8341,7 +8342,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A103" s="42" t="s">
         <v>159</v>
       </c>
@@ -8370,7 +8371,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="42" t="s">
         <v>159</v>
       </c>
@@ -9849,7 +9850,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="155" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A155" s="42" t="s">
         <v>217</v>
       </c>
@@ -9878,7 +9879,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="156" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A156" s="42" t="s">
         <v>217</v>
       </c>
@@ -9907,7 +9908,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="157" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A157" s="42" t="s">
         <v>217</v>
       </c>
@@ -9936,7 +9937,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="158" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A158" s="42" t="s">
         <v>217</v>
       </c>
@@ -9965,7 +9966,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="159" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A159" s="42" t="s">
         <v>217</v>
       </c>
@@ -9994,7 +9995,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="160" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A160" s="42" t="s">
         <v>217</v>
       </c>
@@ -10023,7 +10024,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="161" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A161" s="42" t="s">
         <v>217</v>
       </c>
@@ -10052,7 +10053,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="162" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A162" s="42" t="s">
         <v>217</v>
       </c>
@@ -10081,7 +10082,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="163" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A163" s="42" t="s">
         <v>217</v>
       </c>
@@ -10110,7 +10111,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="164" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A164" s="42" t="s">
         <v>217</v>
       </c>
@@ -10139,7 +10140,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="165" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A165" s="42" t="s">
         <v>217</v>
       </c>
@@ -10168,7 +10169,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="166" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A166" s="42" t="s">
         <v>217</v>
       </c>
@@ -10197,7 +10198,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="167" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A167" s="42" t="s">
         <v>217</v>
       </c>
@@ -10226,7 +10227,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="168" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A168" s="42" t="s">
         <v>217</v>
       </c>
@@ -10255,7 +10256,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="169" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A169" s="42" t="s">
         <v>217</v>
       </c>
@@ -10284,7 +10285,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="170" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A170" s="42" t="s">
         <v>217</v>
       </c>
@@ -10313,7 +10314,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="171" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A171" s="42" t="s">
         <v>217</v>
       </c>
@@ -10342,7 +10343,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="172" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A172" s="42" t="s">
         <v>217</v>
       </c>
@@ -10371,7 +10372,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="173" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A173" s="42" t="s">
         <v>217</v>
       </c>
@@ -10400,7 +10401,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="174" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A174" s="42" t="s">
         <v>217</v>
       </c>
@@ -10429,7 +10430,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="175" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A175" s="42" t="s">
         <v>217</v>
       </c>
@@ -10458,7 +10459,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="176" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A176" s="42" t="s">
         <v>217</v>
       </c>
@@ -10487,7 +10488,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="177" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A177" s="42" t="s">
         <v>217</v>
       </c>
@@ -10516,7 +10517,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="178" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A178" s="42" t="s">
         <v>217</v>
       </c>
@@ -10545,7 +10546,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="179" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A179" s="42" t="s">
         <v>217</v>
       </c>
@@ -10574,7 +10575,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="180" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A180" s="42" t="s">
         <v>217</v>
       </c>
@@ -10603,7 +10604,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="181" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A181" s="42" t="s">
         <v>217</v>
       </c>
@@ -10719,7 +10720,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="185" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A185" s="42" t="s">
         <v>217</v>
       </c>
@@ -10806,7 +10807,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="188" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A188" s="42" t="s">
         <v>217</v>
       </c>
@@ -10835,7 +10836,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="189" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A189" s="42" t="s">
         <v>217</v>
       </c>
@@ -10864,7 +10865,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="190" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A190" s="42" t="s">
         <v>217</v>
       </c>
@@ -10893,7 +10894,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="191" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A191" s="42" t="s">
         <v>217</v>
       </c>
@@ -10922,7 +10923,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="192" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A192" s="42" t="s">
         <v>217</v>
       </c>
@@ -10951,7 +10952,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="193" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A193" s="42" t="s">
         <v>217</v>
       </c>
@@ -10980,7 +10981,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="194" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A194" s="42" t="s">
         <v>217</v>
       </c>
@@ -11009,7 +11010,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="195" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A195" s="42" t="s">
         <v>217</v>
       </c>
@@ -11038,7 +11039,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="196" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A196" s="42" t="s">
         <v>217</v>
       </c>
@@ -11067,7 +11068,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="197" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A197" s="42" t="s">
         <v>217</v>
       </c>
@@ -11125,7 +11126,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="199" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A199" s="42" t="s">
         <v>217</v>
       </c>
@@ -11183,7 +11184,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="201" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A201" s="42" t="s">
         <v>217</v>
       </c>
@@ -11792,7 +11793,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="222" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222" s="42" t="s">
         <v>310</v>
       </c>
@@ -11821,7 +11822,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="223" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A223" s="42" t="s">
         <v>310</v>
       </c>
@@ -12111,7 +12112,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="233" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:9" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A233" s="42" t="s">
         <v>310</v>
       </c>
@@ -14576,7 +14577,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="318" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A318" s="42" t="s">
         <v>436</v>
       </c>
@@ -17099,7 +17100,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="405" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A405" s="42" t="s">
         <v>570</v>
       </c>
@@ -17157,7 +17158,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="407" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A407" s="42" t="s">
         <v>570</v>
       </c>
@@ -17186,7 +17187,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="408" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A408" s="42" t="s">
         <v>570</v>
       </c>
@@ -17215,7 +17216,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="409" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A409" s="42" t="s">
         <v>570</v>
       </c>
@@ -17244,7 +17245,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="410" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A410" s="42" t="s">
         <v>570</v>
       </c>
@@ -17273,7 +17274,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="411" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A411" s="42" t="s">
         <v>570</v>
       </c>
@@ -17302,7 +17303,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="412" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="412" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A412" s="42" t="s">
         <v>570</v>
       </c>
@@ -17331,7 +17332,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="413" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="413" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A413" s="42" t="s">
         <v>570</v>
       </c>
@@ -17360,7 +17361,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="414" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A414" s="42" t="s">
         <v>570</v>
       </c>
@@ -17389,7 +17390,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="415" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="415" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A415" s="42" t="s">
         <v>570</v>
       </c>
@@ -17418,7 +17419,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="416" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:9" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A416" s="42" t="s">
         <v>570</v>
       </c>
@@ -17447,7 +17448,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="417" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A417" s="42" t="s">
         <v>570</v>
       </c>
@@ -17476,7 +17477,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="418" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:9" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A418" s="42" t="s">
         <v>570</v>
       </c>
@@ -17563,7 +17564,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="421" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:9" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A421" s="42" t="s">
         <v>570</v>
       </c>
@@ -17592,7 +17593,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="422" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A422" s="42" t="s">
         <v>570</v>
       </c>
@@ -17621,7 +17622,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="423" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A423" s="42" t="s">
         <v>570</v>
       </c>
@@ -17679,7 +17680,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="425" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A425" s="42" t="s">
         <v>570</v>
       </c>
@@ -17911,7 +17912,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="433" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A433" s="42" t="s">
         <v>625</v>
       </c>
@@ -17940,7 +17941,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="434" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="434" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A434" s="42" t="s">
         <v>625</v>
       </c>
@@ -17969,7 +17970,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="435" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A435" s="42" t="s">
         <v>625</v>
       </c>
@@ -17998,7 +17999,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="436" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A436" s="42" t="s">
         <v>625</v>
       </c>
@@ -18027,7 +18028,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="437" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A437" s="42" t="s">
         <v>625</v>
       </c>
@@ -18056,7 +18057,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="438" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="438" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A438" s="42" t="s">
         <v>625</v>
       </c>
@@ -18085,7 +18086,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="439" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A439" s="42" t="s">
         <v>625</v>
       </c>
@@ -18114,7 +18115,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="440" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A440" s="42" t="s">
         <v>625</v>
       </c>
@@ -18143,7 +18144,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="441" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A441" s="42" t="s">
         <v>625</v>
       </c>
@@ -18172,7 +18173,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="442" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="442" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A442" s="42" t="s">
         <v>625</v>
       </c>
@@ -18201,7 +18202,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="443" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A443" s="42" t="s">
         <v>625</v>
       </c>
@@ -18230,7 +18231,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="444" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A444" s="42" t="s">
         <v>625</v>
       </c>
@@ -18259,7 +18260,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="445" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A445" s="42" t="s">
         <v>625</v>
       </c>
@@ -18288,7 +18289,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="446" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A446" s="42" t="s">
         <v>625</v>
       </c>
@@ -18317,7 +18318,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="447" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="447" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A447" s="42" t="s">
         <v>625</v>
       </c>
@@ -18346,7 +18347,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="448" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A448" s="42" t="s">
         <v>625</v>
       </c>
@@ -18375,7 +18376,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="449" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A449" s="42" t="s">
         <v>625</v>
       </c>
@@ -18404,7 +18405,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="450" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A450" s="42" t="s">
         <v>625</v>
       </c>
@@ -18433,7 +18434,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="451" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A451" s="42" t="s">
         <v>625</v>
       </c>
@@ -18462,7 +18463,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="452" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A452" s="42" t="s">
         <v>625</v>
       </c>
@@ -18491,7 +18492,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="453" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="453" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A453" s="42" t="s">
         <v>625</v>
       </c>
@@ -18520,7 +18521,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="454" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A454" s="42" t="s">
         <v>625</v>
       </c>
@@ -18549,7 +18550,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="455" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A455" s="42" t="s">
         <v>625</v>
       </c>
@@ -18578,7 +18579,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="456" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A456" s="42" t="s">
         <v>625</v>
       </c>
@@ -18607,7 +18608,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="457" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A457" s="42" t="s">
         <v>625</v>
       </c>
@@ -18636,7 +18637,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="458" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A458" s="42" t="s">
         <v>625</v>
       </c>
@@ -18665,7 +18666,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="459" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A459" s="42" t="s">
         <v>625</v>
       </c>
@@ -18694,7 +18695,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="460" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="460" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A460" s="42" t="s">
         <v>625</v>
       </c>
@@ -18723,7 +18724,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="461" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A461" s="42" t="s">
         <v>625</v>
       </c>
@@ -18752,7 +18753,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="462" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="462" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A462" s="42" t="s">
         <v>625</v>
       </c>
@@ -18781,7 +18782,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="463" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A463" s="42" t="s">
         <v>625</v>
       </c>
@@ -18810,7 +18811,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="464" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A464" s="42" t="s">
         <v>625</v>
       </c>
@@ -18839,7 +18840,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="465" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A465" s="42" t="s">
         <v>625</v>
       </c>
@@ -18868,7 +18869,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="466" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A466" s="42" t="s">
         <v>625</v>
       </c>
@@ -18926,7 +18927,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="468" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="468" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A468" s="42" t="s">
         <v>625</v>
       </c>
@@ -18955,7 +18956,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="469" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A469" s="42" t="s">
         <v>625</v>
       </c>
@@ -18984,7 +18985,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="470" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A470" s="42" t="s">
         <v>625</v>
       </c>
@@ -19013,7 +19014,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="471" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="471" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A471" s="42" t="s">
         <v>625</v>
       </c>
@@ -19042,7 +19043,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="472" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A472" s="42" t="s">
         <v>625</v>
       </c>
@@ -19071,7 +19072,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="473" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A473" s="42" t="s">
         <v>625</v>
       </c>
@@ -19100,7 +19101,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="474" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A474" s="42" t="s">
         <v>625</v>
       </c>
@@ -19129,7 +19130,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="475" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A475" s="42" t="s">
         <v>625</v>
       </c>
@@ -19158,7 +19159,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="476" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A476" s="42" t="s">
         <v>625</v>
       </c>
@@ -19187,7 +19188,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="477" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A477" s="42" t="s">
         <v>625</v>
       </c>
@@ -19216,7 +19217,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="478" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A478" s="42" t="s">
         <v>625</v>
       </c>
@@ -19245,7 +19246,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="479" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="479" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A479" s="42" t="s">
         <v>625</v>
       </c>
@@ -19274,7 +19275,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="480" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="480" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A480" s="42" t="s">
         <v>625</v>
       </c>
@@ -19303,7 +19304,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="481" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A481" s="42" t="s">
         <v>640</v>
       </c>
@@ -19332,7 +19333,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="482" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:9" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A482" s="42" t="s">
         <v>640</v>
       </c>
@@ -19361,7 +19362,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="483" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="483" spans="1:9" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A483" s="42" t="s">
         <v>640</v>
       </c>
@@ -19390,7 +19391,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="484" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="484" spans="1:9" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A484" s="42" t="s">
         <v>640</v>
       </c>
@@ -19419,7 +19420,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="485" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="485" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A485" s="42" t="s">
         <v>640</v>
       </c>
@@ -19448,7 +19449,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="486" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A486" s="42" t="s">
         <v>640</v>
       </c>
@@ -19477,7 +19478,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="487" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A487" s="42" t="s">
         <v>640</v>
       </c>
@@ -19506,7 +19507,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="488" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A488" s="42" t="s">
         <v>640</v>
       </c>
@@ -19535,7 +19536,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="489" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A489" s="42" t="s">
         <v>640</v>
       </c>
@@ -19564,7 +19565,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="490" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A490" s="42" t="s">
         <v>640</v>
       </c>
@@ -19593,7 +19594,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="491" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A491" s="42" t="s">
         <v>640</v>
       </c>
@@ -19622,7 +19623,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="492" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A492" s="42" t="s">
         <v>640</v>
       </c>
@@ -19651,7 +19652,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="493" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="493" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A493" s="42" t="s">
         <v>645</v>
       </c>
@@ -19680,7 +19681,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="494" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A494" s="42" t="s">
         <v>645</v>
       </c>
@@ -19709,7 +19710,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="495" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A495" s="42" t="s">
         <v>645</v>
       </c>
@@ -19738,7 +19739,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="496" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A496" s="42" t="s">
         <v>645</v>
       </c>
@@ -19767,7 +19768,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="497" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A497" s="42" t="s">
         <v>645</v>
       </c>
@@ -19796,7 +19797,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="498" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A498" s="42" t="s">
         <v>645</v>
       </c>
@@ -19825,7 +19826,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="499" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A499" s="42" t="s">
         <v>645</v>
       </c>
@@ -19854,7 +19855,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="500" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A500" s="42" t="s">
         <v>645</v>
       </c>
@@ -19883,7 +19884,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="501" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A501" s="42" t="s">
         <v>645</v>
       </c>
@@ -19912,7 +19913,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="502" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A502" s="42" t="s">
         <v>645</v>
       </c>
@@ -19941,7 +19942,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="503" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A503" s="42" t="s">
         <v>645</v>
       </c>
@@ -19970,7 +19971,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="504" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A504" s="42" t="s">
         <v>645</v>
       </c>
@@ -19999,7 +20000,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="505" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A505" s="42" t="s">
         <v>645</v>
       </c>
@@ -20028,7 +20029,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="506" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A506" s="42" t="s">
         <v>645</v>
       </c>
@@ -20057,7 +20058,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="507" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A507" s="42" t="s">
         <v>645</v>
       </c>
@@ -20086,7 +20087,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="508" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A508" s="42" t="s">
         <v>645</v>
       </c>
@@ -20115,7 +20116,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="509" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A509" s="42" t="s">
         <v>645</v>
       </c>
@@ -20144,7 +20145,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="510" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A510" s="42" t="s">
         <v>645</v>
       </c>
@@ -20173,7 +20174,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="511" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A511" s="42" t="s">
         <v>645</v>
       </c>
@@ -20202,7 +20203,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="512" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A512" s="42" t="s">
         <v>645</v>
       </c>
@@ -20260,7 +20261,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="514" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A514" s="42" t="s">
         <v>645</v>
       </c>
@@ -20289,7 +20290,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="515" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A515" s="42" t="s">
         <v>645</v>
       </c>
@@ -20318,7 +20319,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="516" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="516" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A516" s="42" t="s">
         <v>645</v>
       </c>
@@ -20347,7 +20348,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="517" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A517" s="42" t="s">
         <v>645</v>
       </c>
@@ -20376,7 +20377,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="518" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="518" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A518" s="42" t="s">
         <v>645</v>
       </c>
@@ -20405,7 +20406,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="519" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A519" s="42" t="s">
         <v>652</v>
       </c>
@@ -20434,7 +20435,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="520" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A520" s="42" t="s">
         <v>652</v>
       </c>
@@ -20463,7 +20464,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="521" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A521" s="42" t="s">
         <v>652</v>
       </c>
@@ -20492,7 +20493,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="522" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A522" s="42" t="s">
         <v>652</v>
       </c>
@@ -20521,7 +20522,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="523" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A523" s="42" t="s">
         <v>652</v>
       </c>
@@ -20550,7 +20551,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="524" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A524" s="42" t="s">
         <v>652</v>
       </c>
@@ -20579,7 +20580,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="525" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A525" s="42" t="s">
         <v>652</v>
       </c>
@@ -26727,7 +26728,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="737" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="737" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A737" s="42" t="s">
         <v>916</v>
       </c>
@@ -26756,7 +26757,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="738" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="738" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A738" s="42" t="s">
         <v>916</v>
       </c>
@@ -26785,7 +26786,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="739" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="739" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A739" s="42" t="s">
         <v>916</v>
       </c>
@@ -26814,7 +26815,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="740" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="740" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A740" s="42" t="s">
         <v>916</v>
       </c>
@@ -26872,7 +26873,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="742" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="742" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A742" s="42" t="s">
         <v>916</v>
       </c>
@@ -26901,7 +26902,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="743" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="743" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A743" s="42" t="s">
         <v>916</v>
       </c>
@@ -26930,7 +26931,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="744" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="744" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A744" s="42" t="s">
         <v>916</v>
       </c>
@@ -26988,7 +26989,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="746" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="746" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A746" s="42" t="s">
         <v>916</v>
       </c>
@@ -27017,7 +27018,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="747" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="747" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A747" s="42" t="s">
         <v>916</v>
       </c>
@@ -27046,7 +27047,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="748" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="748" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A748" s="42" t="s">
         <v>916</v>
       </c>
@@ -27104,7 +27105,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="750" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="750" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A750" s="42" t="s">
         <v>916</v>
       </c>
@@ -27133,7 +27134,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="751" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="751" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A751" s="42" t="s">
         <v>916</v>
       </c>
@@ -27162,7 +27163,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="752" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="752" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A752" s="42" t="s">
         <v>916</v>
       </c>
@@ -27191,7 +27192,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="753" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="753" spans="1:9" ht="57" x14ac:dyDescent="0.25">
       <c r="A753" s="42" t="s">
         <v>916</v>
       </c>
@@ -27220,7 +27221,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="754" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="754" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A754" s="42" t="s">
         <v>916</v>
       </c>
@@ -27249,7 +27250,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="755" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="755" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A755" s="42" t="s">
         <v>916</v>
       </c>
@@ -27278,7 +27279,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="756" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="756" spans="1:9" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A756" s="42" t="s">
         <v>916</v>
       </c>
@@ -30149,7 +30150,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="855" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="855" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A855" s="6" t="s">
         <v>1068</v>
       </c>
@@ -30178,7 +30179,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="856" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="856" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A856" s="6" t="s">
         <v>1068</v>
       </c>
@@ -30207,7 +30208,7 @@
         <v>1072</v>
       </c>
     </row>
-    <row r="857" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="857" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A857" s="6" t="s">
         <v>1068</v>
       </c>
@@ -30236,7 +30237,7 @@
         <v>1073</v>
       </c>
     </row>
-    <row r="858" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="858" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A858" s="6" t="s">
         <v>1068</v>
       </c>
@@ -30265,7 +30266,7 @@
         <v>1074</v>
       </c>
     </row>
-    <row r="859" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="859" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A859" s="6" t="s">
         <v>1068</v>
       </c>
@@ -30294,7 +30295,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="860" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="860" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A860" s="6" t="s">
         <v>1068</v>
       </c>
@@ -30323,7 +30324,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="861" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="861" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A861" s="6" t="s">
         <v>1068</v>
       </c>
@@ -30352,7 +30353,7 @@
         <v>1079</v>
       </c>
     </row>
-    <row r="862" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="862" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A862" s="6" t="s">
         <v>1068</v>
       </c>
@@ -30381,7 +30382,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="863" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="863" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A863" s="6" t="s">
         <v>1068</v>
       </c>
@@ -30410,7 +30411,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="864" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="864" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A864" s="6" t="s">
         <v>1068</v>
       </c>
@@ -30439,7 +30440,7 @@
         <v>1082</v>
       </c>
     </row>
-    <row r="865" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="865" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A865" s="6" t="s">
         <v>1068</v>
       </c>
@@ -30497,7 +30498,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="867" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="867" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A867" s="6" t="s">
         <v>1068</v>
       </c>
@@ -30526,7 +30527,7 @@
         <v>1087</v>
       </c>
     </row>
-    <row r="868" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="868" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A868" s="6" t="s">
         <v>1068</v>
       </c>
@@ -30555,7 +30556,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="869" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="869" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A869" s="6" t="s">
         <v>1068</v>
       </c>
@@ -30613,7 +30614,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="871" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="871" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A871" s="6" t="s">
         <v>1068</v>
       </c>
@@ -30642,7 +30643,7 @@
         <v>1093</v>
       </c>
     </row>
-    <row r="872" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="872" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A872" s="6" t="s">
         <v>1068</v>
       </c>
@@ -30671,7 +30672,7 @@
         <v>1095</v>
       </c>
     </row>
-    <row r="873" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="873" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A873" s="6" t="s">
         <v>1068</v>
       </c>
@@ -30700,7 +30701,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="874" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="874" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A874" s="6" t="s">
         <v>1068</v>
       </c>
@@ -30729,7 +30730,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="875" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="875" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A875" s="6" t="s">
         <v>1068</v>
       </c>
@@ -30758,7 +30759,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="876" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="876" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A876" s="6" t="s">
         <v>1068</v>
       </c>
@@ -30787,7 +30788,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="877" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="877" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A877" s="6" t="s">
         <v>1068</v>
       </c>
@@ -30816,7 +30817,7 @@
         <v>1101</v>
       </c>
     </row>
-    <row r="878" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="878" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A878" s="6" t="s">
         <v>1068</v>
       </c>
@@ -31773,7 +31774,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="911" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="911" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A911" s="6" t="s">
         <v>1143</v>
       </c>
@@ -31802,7 +31803,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="912" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="912" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A912" s="6" t="s">
         <v>1143</v>
       </c>
@@ -31831,7 +31832,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="913" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="913" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A913" s="6" t="s">
         <v>1143</v>
       </c>
@@ -31860,7 +31861,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="914" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="914" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A914" s="6" t="s">
         <v>1143</v>
       </c>
@@ -31889,7 +31890,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="915" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="915" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A915" s="6" t="s">
         <v>1143</v>
       </c>
@@ -31918,7 +31919,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="916" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="916" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A916" s="6" t="s">
         <v>1143</v>
       </c>
@@ -31947,7 +31948,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="917" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="917" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A917" s="6" t="s">
         <v>1143</v>
       </c>
@@ -31976,7 +31977,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="918" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="918" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A918" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32005,7 +32006,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="919" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="919" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A919" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32034,7 +32035,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="920" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="920" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A920" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32063,7 +32064,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="921" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="921" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A921" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32092,7 +32093,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="922" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="922" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A922" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32121,7 +32122,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="923" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="923" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A923" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32150,7 +32151,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="924" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="924" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A924" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32179,7 +32180,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="925" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="925" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A925" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32208,7 +32209,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="926" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="926" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A926" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32237,7 +32238,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="927" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="927" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A927" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32266,7 +32267,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="928" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="928" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A928" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32295,7 +32296,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="929" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="929" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A929" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32324,7 +32325,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="930" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="930" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A930" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32353,7 +32354,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="931" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="931" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A931" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32382,7 +32383,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="932" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="932" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A932" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32411,7 +32412,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="933" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="933" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A933" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32440,7 +32441,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="934" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="934" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A934" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32469,7 +32470,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="935" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="935" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A935" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32498,7 +32499,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="936" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="936" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A936" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32527,7 +32528,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="937" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="937" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A937" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32556,7 +32557,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="938" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="938" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A938" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32585,7 +32586,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="939" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="939" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A939" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32614,7 +32615,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="940" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="940" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A940" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32643,7 +32644,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="941" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="941" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A941" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32672,7 +32673,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="942" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="942" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A942" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32701,7 +32702,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="943" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="943" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A943" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32730,7 +32731,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="944" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="944" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A944" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32759,7 +32760,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="945" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="945" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A945" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32788,7 +32789,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="946" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="946" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A946" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32817,7 +32818,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="947" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="947" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A947" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32846,7 +32847,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="948" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="948" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A948" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32875,7 +32876,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="949" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="949" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A949" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32904,7 +32905,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="950" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="950" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A950" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32933,7 +32934,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="951" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="951" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A951" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32962,7 +32963,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="952" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="952" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A952" s="6" t="s">
         <v>1143</v>
       </c>
@@ -32991,7 +32992,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="953" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="953" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A953" s="6" t="s">
         <v>1143</v>
       </c>
@@ -33020,7 +33021,7 @@
         <v>1146</v>
       </c>
     </row>
-    <row r="954" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="954" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A954" s="6" t="s">
         <v>1143</v>
       </c>

</xml_diff>